<commit_message>
fix the "one cent diff" bug
</commit_message>
<xml_diff>
--- a/www/categories.xlsx
+++ b/www/categories.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,11 +20,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="674">
   <si>
     <t xml:space="preserve">Fruits &amp; Légumes</t>
   </si>
   <si>
+    <t xml:space="preserve">Paniers composés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panier de fruits et légumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panier de légumes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panier de fruits</t>
+  </si>
+  <si>
     <t xml:space="preserve">Légumes</t>
   </si>
   <si>
@@ -94,27 +115,6 @@
     <t xml:space="preserve">Légumes tiges</t>
   </si>
   <si>
-    <t xml:space="preserve">Paniers composés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">157</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panier de fruits et légumes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">158</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panier de légumes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">350</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Panier de fruits</t>
-  </si>
-  <si>
     <t xml:space="preserve">Fruits</t>
   </si>
   <si>
@@ -928,6 +928,9 @@
     <t xml:space="preserve">Oeufs</t>
   </si>
   <si>
+    <t xml:space="preserve">Paniers composés et fromages mixtes</t>
+  </si>
+  <si>
     <t xml:space="preserve">666</t>
   </si>
   <si>
@@ -937,6 +940,12 @@
     <t xml:space="preserve">paniers composés</t>
   </si>
   <si>
+    <t xml:space="preserve">800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fromages mixtes</t>
+  </si>
+  <si>
     <t xml:space="preserve">Boulangerie et pâtisserie</t>
   </si>
   <si>
@@ -1213,6 +1222,12 @@
     <t xml:space="preserve">Conserves de viande</t>
   </si>
   <si>
+    <t xml:space="preserve">802</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conserves lacto-fermentées</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pâtes et riz</t>
   </si>
   <si>
@@ -1441,6 +1456,9 @@
     <t xml:space="preserve">Graines</t>
   </si>
   <si>
+    <t xml:space="preserve">799</t>
+  </si>
+  <si>
     <t xml:space="preserve">Confitures et autres tartinables</t>
   </si>
   <si>
@@ -1870,6 +1888,12 @@
     <t xml:space="preserve">Autres compléments</t>
   </si>
   <si>
+    <t xml:space="preserve">801</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gemmothérapie</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plants et autres</t>
   </si>
   <si>
@@ -2003,6 +2027,606 @@
   </si>
   <si>
     <t xml:space="preserve">Frais autres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">charset=UTF-8" xml:lang="fr" lang="fr"/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;/span&gt;&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&gt;
+                    &lt;button type="button" class="btn btn-default" data-dismiss="modal"&gt;
+                        &lt;i class="icon icon-delete"&gt;&lt;/i&gt; Fermer
+                    &lt;/button&gt;
+                &lt;/div&gt;
+            &lt;/div&gt;
+        &lt;/div&gt;
+    &lt;/div&gt;
+		&lt;div class="row header" style="margin-top:10px;"&gt;
+			&lt;div class="col-md-8"&gt;
+					&lt;h1&gt;AMAP du petit Chantilly - Orvault&lt;/h1&gt;
+			&lt;/div&gt;
+			&lt;div class="col-md-4 accountBlock"&gt;					
+			&lt;!-- Home --&gt;			
+			&lt;div class="dropdown pull-right text-right"&gt;
+				&lt;a class="dropdown-toggle" type="button" id="dropdownMenuUser" data-toggle="dropdown"&gt;
+					&lt;i class="icon icon-user"&gt;&lt;/i&gt;
+					BARBUT François
+				&lt;/a&gt;
+				&lt;ul class="dropdown-menu dropdown-menu-right" aria-labelledby="dropdownMenuUser"&gt;
+					&lt;li&gt;&lt;a href="/admin"&gt;&lt;i class="icon icon-cog"&gt;&lt;/i&gt; Admin&lt;/a&gt;&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/db"&gt;&lt;i class="icon icon-cog"&gt;&lt;/i&gt; Base de données&lt;/a&gt;&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/user/logout"&gt;&lt;i class="icon icon-delete"&gt;&lt;/i&gt; Déconnexion&lt;/a&gt;&lt;/li&gt;
+				&lt;/ul&gt;
+			&lt;/div&gt;			
+		&lt;!-- Help --&gt;
+		&lt;div class="dropdown pull-right text-right" id="helpMenu"&gt;
+			&lt;a class="dropdown-toggle" type="button" id="dropdownMenuHelp" data-toggle="dropdown"&gt;
+				&lt;i class="icon icon-info"&gt;&lt;/i&gt; Aide
+			&lt;/a&gt;
+			&lt;ul class="dropdown-menu dropdown-menu-right" aria-labelledby="dropdownMenuHelp"&gt;
+				&lt;li&gt;
+					&lt;a href="http://wiki.cagette.net" target="_blank"&gt;&lt;i class="icon icon-book"&gt;&lt;/i&gt; Documentation&lt;/a&gt; 
+				&lt;/li&gt;
+				&lt;li&gt;
+					&lt;a href="https://www.facebook.com/groups/EntraideCagette/" target="_blank"&gt;&lt;i class="icon icon-facebook"&gt;&lt;/i&gt; Groupe Facebook&lt;/a&gt; 
+				&lt;/li&gt;
+				&lt;li&gt;
+					&lt;a href="http://www.cagette.pro" target="_blank"&gt;&lt;i class="icon icon-student"&gt;&lt;/i&gt; Formations pour producteurs&lt;/a&gt; 
+				&lt;/li&gt;				
+			&lt;/ul&gt;
+		&lt;/div&gt;
+		&lt;!-- Home --&gt;
+		&lt;div class="pull-right"&gt;
+			&lt;a class=" href="/user/choose?show=1"&gt;
+				&lt;i class="icon icon-chevron-left"&gt;&lt;/i&gt; Accueil
+			&lt;/a&gt;
+		&lt;/div&gt;
+			&lt;/div&gt;				
+		&lt;/div&gt;
+			&lt;nav class="navbar navbar-default"&gt;
+					&lt;div class="navbar-header"&gt;
+					  &lt;button type="button" class="navbar-toggle collapsed" data-toggle="collapse" data-target="#cagette-navbar"&gt;
+						&lt;span class="sr-only"&gt;Toggle navigation&lt;/span&gt;						
+						&lt;span class="icon-bar"&gt;&lt;/span&gt;
+						&lt;span class="icon-bar"&gt;&lt;/span&gt;
+						&lt;span class="icon-bar"&gt;&lt;/span&gt;
+					  &lt;/button&gt;				  
+					&lt;/div&gt;	
+					&lt;div class="collapse navbar-collapse" id="cagette-navbar"&gt;
+						&lt;ul class="nav navbar-nav navbar-left"&gt;
+							&lt;li&gt;
+								&lt;a href="/"&gt;
+									&lt;i class="icon icon-basket"&gt;&lt;/i&gt;  Commandes
+								&lt;/a&gt;
+							&lt;/li&gt;
+							&lt;li&gt;
+								&lt;a href="/account"&gt;
+									&lt;i class="icon icon-user"&gt;&lt;/i&gt; Mon compte
+								&lt;/a&gt;
+							&lt;/li&gt;
+							&lt;li&gt;
+								&lt;a href="/amap"&gt;
+									&lt;i class="icon icon-farmer"&gt;&lt;/i&gt; Producteurs
+								&lt;/a&gt;
+							&lt;/li&gt;
+						&lt;/ul&gt;
+						&lt;ul class="nav navbar-nav navbar-right admin"&gt;
+							&lt;li id="member"&gt;								
+								&lt;a href="/member"&gt;
+									&lt;i class="icon icon-users"&gt;&lt;/i&gt; Membres
+								&lt;/a&gt;
+							&lt;/li&gt;
+							&lt;li id="distributions"&gt;
+								&lt;a href="/distribution"&gt;
+									&lt;i class="icon icon-calendar"&gt;&lt;/i&gt;  Distributions
+								&lt;/a&gt;
+							&lt;/li&gt;
+							&lt;li id="contractadmin"&gt;
+								&lt;a href="/contractAdmin"&gt;
+									&lt;i class="icon icon-book"&gt;&lt;/i&gt; Catalogues
+								&lt;/a&gt;
+							&lt;/li&gt;
+							&lt;li id="messages"&gt;
+								&lt;a href="/messages"&gt;
+									&lt;i class="icon icon-mail"&gt;&lt;/i&gt;  Messagerie
+								&lt;/a&gt;
+							&lt;/li&gt;
+							&lt;li id="amapadmin"&gt;
+								&lt;a href="/amapadmin"&gt;
+									&lt;i class="icon icon-cog"&gt;&lt;/i&gt;  Paramètres
+								&lt;/a&gt;
+							&lt;/li&gt;							
+						&lt;/ul&gt;
+					&lt;/div&gt;
+			&lt;/nav&gt;
+		&lt;!-- Breadcrumb --&gt;
+		&lt;div class="row"&gt;
+			&lt;div class="col-md-12"&gt;
+				&lt;ol class="breadcrumb"&gt;
+					&lt;li&gt;&lt;a href="/user/choose"&gt;Accueil&lt;/a&gt;&lt;/li&gt;
+						&lt;li id="g3865"&gt;&lt;a href="/home"&gt;Groupe Cagette : AMAP du petit Chantilly - Orvault&lt;/a&gt;&lt;/li&gt;
+				&lt;/ol&gt;
+			&lt;/div&gt;
+		&lt;/div&gt;
+		&lt;!-- Notifications --&gt;
+		&lt;div class="row"&gt;
+			&lt;div id="content" class="col-md-12"&gt;
+			&lt;/div&gt;	
+		&lt;/div&gt;
+		&lt;!-- extra notification block for plugins --&gt;
+		&lt;div class="row"&gt;
+&lt;div class="col-md-3"&gt;
+	&lt;div class="panel panel-warning"&gt;
+		&lt;div class="panel-heading"&gt;
+			&lt;span class="panel-title"&gt;&lt;a href="/admin"&gt;Administration&lt;/a&gt;&lt;/span&gt;
+		&lt;/div&gt;
+		&lt;ul class="nav nav-tabs nav-stacked"&gt;
+			&lt;li&gt;&lt;a href="/db"&gt;&lt;i class="icon icon-cog"&gt;&lt;/i&gt; Base de données&lt;/a&gt; &lt;/li&gt;
+			&lt;li&gt;&lt;a href="/admin/taxo"&gt;&lt;i class="icon icon-tag"&gt;&lt;/i&gt; Catégories&lt;/a&gt; &lt;/li&gt;			
+			&lt;li&gt;&lt;a href="/admin/errors"&gt;&lt;i class="icon icon-cog"&gt;&lt;/i&gt; Errors&lt;/a&gt; &lt;/li&gt;			
+			&lt;!--&lt;li&gt;&lt;a href="/admin/smtp"&gt;&lt;i class="icon icon-mail"&gt;&lt;/i&gt; Conf. Email&lt;/a&gt; &lt;/li&gt;	--&gt;		
+			&lt;li&gt;&lt;a href="/admin/emails"&gt;&lt;i class="icon icon-mail"&gt;&lt;/i&gt; Emails&lt;/a&gt; &lt;/li&gt;			
+			&lt;li&gt;&lt;a href="/admin/graph"&gt;&lt;i class="icon icon-chart"&gt;&lt;/i&gt; Statistiques&lt;/a&gt; &lt;/li&gt;	
+			&lt;li&gt;&lt;a href="/admin/messages"&gt;&lt;i class="icon icon-info"&gt;&lt;/i&gt; Messages&lt;/a&gt; &lt;/li&gt;					
+					&lt;li&gt;&lt;a href="/p/hosted/user"&gt;
+						&lt;i class="icon icon-user"&gt;&lt;/i&gt; 
+						Utilisateurs&lt;/a&gt;
+					&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/p/hosted"&gt;
+						&lt;i class="icon icon-users"&gt;&lt;/i&gt; 
+						Groupes&lt;/a&gt;
+					&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/p/hosted/course"&gt;
+						&lt;i class="icon icon-student"&gt;&lt;/i&gt; 
+						Formations&lt;/a&gt;
+					&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/p/hosted/seo"&gt;
+						&lt;i class="icon icon-cog"&gt;&lt;/i&gt; 
+						Référencement&lt;/a&gt;
+					&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/p/pro/admin"&gt;
+						&lt;i class="icon icon-farmer"&gt;&lt;/i&gt; 
+						Producteurs&lt;/a&gt;
+					&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/p/pro/admin/deduplicate"&gt;
+						&lt;i class="icon icon-farmer"&gt;&lt;/i&gt; 
+						Déduplication Producteurs&lt;/a&gt;
+					&lt;/li&gt;
+					&lt;li&gt;&lt;a href="/p/pro/admin/siret"&gt;
+						&lt;i class="icon icon-farmer"&gt;&lt;/i&gt; 
+						Producteurs Siret&lt;/a&gt;
+					&lt;/li&gt;
+		&lt;/ul&gt;
+	&lt;/div&gt;
+&lt;/div&gt;
+&lt;div class="col-md-9"&gt;
+	&lt;div class="article"&gt;
+		&lt;h2&gt;Dictionnaire de produits&lt;/h2&gt;
+		&lt;p&gt;
+		&lt;a href="?csv=1" class="btn btn-default btn-sm"&gt;&lt;i class="icon icon-download"&gt;&lt;/i&gt; Export Excel/CSV&lt;/a&gt;	
+			&lt;a href="/admin/mergeCategs" class="btn btn-default btn-sm"&gt;Fusion de categ de niveau 3&lt;/a&gt;
+		&lt;/p&gt;
+		&lt;table class="table table-bordered"&gt;
+			&lt;tr&gt;
+				&lt;th&gt;
+					&lt;h4&gt;#6&lt;/h4&gt;
+					&lt;img src="/img/taxo/legumes.png" style="width:120px;"/&gt;
+					&lt;br/&gt;
+					&lt;h4&gt;&lt;a href="/db/TxpCategory/edit/6" target="_blank"&gt;Fruits &amp;amp; Légumes&lt;/a&gt;&lt;/h4&gt;
+				&lt;/th&gt;
+				&lt;td&gt;
+					&lt;p&gt;
+						&lt;b&gt;#37 &lt;a href="/db/TxpSubCategory/edit/37" target="_blank"&gt;Paniers composés&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/157" target="_blank"&gt;#157 Panier de fruits et légumes&lt;/a&gt; (528 produits),
+						 &lt;a href="/db/TxpProduct/edit/158" target="_blank"&gt;#158 Panier de légumes&lt;/a&gt; (2263 produits),
+						 &lt;a href="/db/TxpProduct/edit/350" target="_blank"&gt;#350 Panier de fruits&lt;/a&gt; (262 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#33 &lt;a href="/db/TxpSubCategory/edit/33" target="_blank"&gt;Légumes&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/163" target="_blank"&gt;#163 Graines germées&lt;/a&gt; (188 produits),
+						 &lt;a href="/db/TxpProduct/edit/555" target="_blank"&gt;#555 Courges&lt;/a&gt; (12800 produits),
+						 &lt;a href="/db/TxpProduct/edit/634" target="_blank"&gt;#634 Choux&lt;/a&gt; (6812 produits),
+						 &lt;a href="/db/TxpProduct/edit/727" target="_blank"&gt;#727 Légumes feuilles&lt;/a&gt; (16737 produits),
+						 &lt;a href="/db/TxpProduct/edit/728" target="_blank"&gt;#728 Légumes fleurs&lt;/a&gt; (2873 produits),
+						 &lt;a href="/db/TxpProduct/edit/729" target="_blank"&gt;#729 Légumes fruits&lt;/a&gt; (16917 produits),
+						 &lt;a href="/db/TxpProduct/edit/730" target="_blank"&gt;#730 Légumes à bulbe&lt;/a&gt; (10866 produits),
+						 &lt;a href="/db/TxpProduct/edit/731" target="_blank"&gt;#731 Légumes tubercule&lt;/a&gt; (471 produits),
+						 &lt;a href="/db/TxpProduct/edit/732" target="_blank"&gt;#732 Légumes graines&lt;/a&gt; (2219 produits),
+						 &lt;a href="/db/TxpProduct/edit/733" target="_blank"&gt;#733 Légumes racine&lt;/a&gt; (25867 produits),
+						 &lt;a href="/db/TxpProduct/edit/734" target="_blank"&gt;#734 Légumes tiges&lt;/a&gt; (269 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#39 &lt;a href="/db/TxpSubCategory/edit/39" target="_blank"&gt;Fruits&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/736" target="_blank"&gt;#736 Fruits à noyau&lt;/a&gt; (2750 produits),
+						 &lt;a href="/db/TxpProduct/edit/737" target="_blank"&gt;#737 Fruits à pépin&lt;/a&gt; (14647 produits),
+						 &lt;a href="/db/TxpProduct/edit/738" target="_blank"&gt;#738 Baies et fruits rouges&lt;/a&gt; (2622 produits),
+						 &lt;a href="/db/TxpProduct/edit/739" target="_blank"&gt;#739 Agrumes&lt;/a&gt; (25749 produits),
+						 &lt;a href="/db/TxpProduct/edit/740" target="_blank"&gt;#740 Fruits à coque&lt;/a&gt; (5006 produits),
+						 &lt;a href="/db/TxpProduct/edit/741" target="_blank"&gt;#741 Fruits exotiques&lt;/a&gt; (1453 produits),
+						 &lt;a href="/db/TxpProduct/edit/770" target="_blank"&gt;#770 Fruits tiges&lt;/a&gt; (420 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#65 &lt;a href="/db/TxpSubCategory/edit/65" target="_blank"&gt;Champignons&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/308" target="_blank"&gt;#308 Truffe&lt;/a&gt; (11 produits),
+						 &lt;a href="/db/TxpProduct/edit/588" target="_blank"&gt;#588 Champignon&lt;/a&gt; (969 produits),
+						 &lt;a href="/db/TxpProduct/edit/779" target="_blank"&gt;#779 Champignons cultivés&lt;/a&gt; (57 produits),
+						 &lt;a href="/db/TxpProduct/edit/780" target="_blank"&gt;#780 Champignons cueillis&lt;/a&gt; (4 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#8 &lt;a href="/db/TxpSubCategory/edit/8" target="_blank"&gt;Aromatiques&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/557" target="_blank"&gt;#557 Reine des prés&lt;/a&gt; (7 produits),
+						 &lt;a href="/db/TxpProduct/edit/596" target="_blank"&gt;#596 Autres plantes sauvages&lt;/a&gt; (485 produits),
+						 &lt;a href="/db/TxpProduct/edit/617" target="_blank"&gt;#617 Lavande&lt;/a&gt; (17 produits),
+						 &lt;a href="/db/TxpProduct/edit/625" target="_blank"&gt;#625 Consoude&lt;/a&gt; (36 produits),
+						 &lt;a href="/db/TxpProduct/edit/774" target="_blank"&gt;#774 Herbes&lt;/a&gt; (657 produits),
+						 &lt;a href="/db/TxpProduct/edit/775" target="_blank"&gt;#775 Plantes&lt;/a&gt; (97 produits),
+						 &lt;a href="/db/TxpProduct/edit/776" target="_blank"&gt;#776 Fruits&lt;/a&gt; (1 produits),
+						 &lt;a href="/db/TxpProduct/edit/777" target="_blank"&gt;#777 Feuilles&lt;/a&gt; (7372 produits),
+						 &lt;a href="/db/TxpProduct/edit/778" target="_blank"&gt;#778 Fleurs comestibles&lt;/a&gt; (564 produits),
+					&lt;/p&gt;
+				&lt;/td&gt;
+			&lt;/tr&gt;
+			&lt;tr&gt;
+				&lt;th&gt;
+					&lt;h4&gt;#10&lt;/h4&gt;
+					&lt;img src="/img/taxo/viande.png" style="width:120px;"/&gt;
+					&lt;br/&gt;
+					&lt;h4&gt;&lt;a href="/db/TxpCategory/edit/10" target="_blank"&gt;Viandes et charcuteries&lt;/a&gt;&lt;/h4&gt;
+				&lt;/th&gt;
+				&lt;td&gt;
+					&lt;p&gt;
+						&lt;b&gt;#61 &lt;a href="/db/TxpSubCategory/edit/61" target="_blank"&gt;Porcs&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/504" target="_blank"&gt;#504 Porc&lt;/a&gt; (10022 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#56 &lt;a href="/db/TxpSubCategory/edit/56" target="_blank"&gt;Volailles&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/134" target="_blank"&gt;#134 Lapin&lt;/a&gt; (223 produits),
+						 &lt;a href="/db/TxpProduct/edit/482" target="_blank"&gt;#482 Pigeon&lt;/a&gt; (57 produits),
+						 &lt;a href="/db/TxpProduct/edit/483" target="_blank"&gt;#483 Autruche&lt;/a&gt; (0 produits),
+						 &lt;a href="/db/TxpProduct/edit/485" target="_blank"&gt;#485 Caille&lt;/a&gt; (106 produits),
+						 &lt;a href="/db/TxpProduct/edit/489" target="_blank"&gt;#489 Canard&lt;/a&gt; (2312 produits),
+						 &lt;a href="/db/TxpProduct/edit/490" target="_blank"&gt;#490 Coquelet&lt;/a&gt; (75 produits),
+						 &lt;a href="/db/TxpProduct/edit/493" target="_blank"&gt;#493 Chapon&lt;/a&gt; (354 produits),
+						 &lt;a href="/db/TxpProduct/edit/495" target="_blank"&gt;#495 Oie&lt;/a&gt; (75 produits),
+						 &lt;a href="/db/TxpProduct/edit/498" target="_blank"&gt;#498 Pintade&lt;/a&gt; (1396 produits),
+						 &lt;a href="/db/TxpProduct/edit/499" target="_blank"&gt;#499 Dinde&lt;/a&gt; (354 produits),
+						 &lt;a href="/db/TxpProduct/edit/505" target="_blank"&gt;#505 Poularde&lt;/a&gt; (214 produits),
+						 &lt;a href="/db/TxpProduct/edit/506" target="_blank"&gt;#506 Poule&lt;/a&gt; (293 produits),
+						 &lt;a href="/db/TxpProduct/edit/507" target="_blank"&gt;#507 Poulet&lt;/a&gt; (8915 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#57 &lt;a href="/db/TxpSubCategory/edit/57" target="_blank"&gt;Boeufs&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/484" target="_blank"&gt;#484 Boeuf&lt;/a&gt; (19401 produits),
+						 &lt;a href="/db/TxpProduct/edit/742" target="_blank"&gt;#742 Génisses&lt;/a&gt; (195 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#86 &lt;a href="/db/TxpSubCategory/edit/86" target="_blank"&gt;Veaux&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/520" target="_blank"&gt;#520 Veau&lt;/a&gt; (10682 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#59 &lt;a href="/db/TxpSubCategory/edit/59" target="_blank"&gt;Ovins&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/90" target="_blank"&gt;#90 Mouton&lt;/a&gt; (1448 produits),
+						 &lt;a href="/db/TxpProduct/edit/500" target="_blank"&gt;#500 Agneau&lt;/a&gt; (8365 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#89 &lt;a href="/db/TxpSubCategory/edit/89" target="_blank"&gt;Caprins&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/680" target="_blank"&gt;#680 Cabri&lt;/a&gt; (89 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#87 &lt;a href="/db/TxpSubCategory/edit/87" target="_blank"&gt;Gibiers&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/491" target="_blank"&gt;#491 Faisan&lt;/a&gt; (1 produits),
+						 &lt;a href="/db/TxpProduct/edit/497" target="_blank"&gt;#497 Perdrix&lt;/a&gt; (0 produits),
+						 &lt;a href="/db/TxpProduct/edit/503" target="_blank"&gt;#503 Cerf&lt;/a&gt; (19 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#16 &lt;a href="/db/TxpSubCategory/edit/16" target="_blank"&gt;Escargots&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/29" target="_blank"&gt;#29 Escargots&lt;/a&gt; (923 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#14 &lt;a href="/db/TxpSubCategory/edit/14" target="_blank"&gt;Autres viandes&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/23" target="_blank"&gt;#23 Bison&lt;/a&gt; (2166 produits),
+						 &lt;a href="/db/TxpProduct/edit/78" target="_blank"&gt;#78 Cheval&lt;/a&gt; (2 produits),
+						 &lt;a href="/db/TxpProduct/edit/79" target="_blank"&gt;#79 Chevreau&lt;/a&gt; (487 produits),
+						 &lt;a href="/db/TxpProduct/edit/189" target="_blank"&gt;#189 Assortiment de viandes&lt;/a&gt; (643 produits),
+						 &lt;a href="/db/TxpProduct/edit/522" target="_blank"&gt;#522 Abats&lt;/a&gt; (672 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#60 &lt;a href="/db/TxpSubCategory/edit/60" target="_blank"&gt;Charcuteries&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/743" target="_blank"&gt;#743 Charcuterie fraiche&lt;/a&gt; (4576 produits),
+						 &lt;a href="/db/TxpProduct/edit/744" target="_blank"&gt;#744 Charcuteries sèches&lt;/a&gt; (2974 produits),
+						 &lt;a href="/db/TxpProduct/edit/745" target="_blank"&gt;#745 Charcuteries fumées&lt;/a&gt; (161 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#36 &lt;a href="/db/TxpSubCategory/edit/36" target="_blank"&gt;Rillettes et pâtés&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/144" target="_blank"&gt;#144 Pâté en croute&lt;/a&gt; (610 produits),
+						 &lt;a href="/db/TxpProduct/edit/155" target="_blank"&gt;#155 Pâté&lt;/a&gt; (3437 produits),
+						 &lt;a href="/db/TxpProduct/edit/190" target="_blank"&gt;#190 Rillettes&lt;/a&gt; (1576 produits),
+						 &lt;a href="/db/TxpProduct/edit/196" target="_blank"&gt;#196 Terrine&lt;/a&gt; (1522 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#58 &lt;a href="/db/TxpSubCategory/edit/58" target="_blank"&gt;Foie gras et confits&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/486" target="_blank"&gt;#486 Confit&lt;/a&gt; (1644 produits),
+						 &lt;a href="/db/TxpProduct/edit/494" target="_blank"&gt;#494 Foie gras&lt;/a&gt; (1663 produits),
+						 &lt;a href="/db/TxpProduct/edit/501" target="_blank"&gt;#501 Magret&lt;/a&gt; (166 produits),
+						 &lt;a href="/db/TxpProduct/edit/509" target="_blank"&gt;#509 Pâté&lt;/a&gt; (151 produits),
+					&lt;/p&gt;
+				&lt;/td&gt;
+			&lt;/tr&gt;
+			&lt;tr&gt;
+				&lt;th&gt;
+					&lt;h4&gt;#1&lt;/h4&gt;
+					&lt;img src="/img/taxo/poisson.png" style="width:120px;"/&gt;
+					&lt;br/&gt;
+					&lt;h4&gt;&lt;a href="/db/TxpCategory/edit/1" target="_blank"&gt;Produits de la mer et d'eau douce&lt;/a&gt;&lt;/h4&gt;
+				&lt;/th&gt;
+				&lt;td&gt;
+					&lt;p&gt;
+						&lt;b&gt;#88 &lt;a href="/db/TxpSubCategory/edit/88" target="_blank"&gt;Poissons&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/1" target="_blank"&gt;#1 Poissons de mer&lt;/a&gt; (2358 produits),
+						 &lt;a href="/db/TxpProduct/edit/184" target="_blank"&gt;#184 Oeufs de poisson&lt;/a&gt; (16 produits),
+						 &lt;a href="/db/TxpProduct/edit/245" target="_blank"&gt;#245 Poissons d'eau douce&lt;/a&gt; (479 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#12 &lt;a href="/db/TxpSubCategory/edit/12" target="_blank"&gt;Coquillages et crustacés&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/21" target="_blank"&gt;#21 Coquillages&lt;/a&gt; (550 produits),
+						 &lt;a href="/db/TxpProduct/edit/170" target="_blank"&gt;#170 Céphalopodes&lt;/a&gt; (37 produits),
+						 &lt;a href="/db/TxpProduct/edit/224" target="_blank"&gt;#224 Crustacés&lt;/a&gt; (63 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#44 &lt;a href="/db/TxpSubCategory/edit/44" target="_blank"&gt;Soupes et Rillettes&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/682" target="_blank"&gt;#682 Rillettes de poisson&lt;/a&gt; (744 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#15 &lt;a href="/db/TxpSubCategory/edit/15" target="_blank"&gt;Algues&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/24" target="_blank"&gt;#24 Algues&lt;/a&gt; (110 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#74 &lt;a href="/db/TxpSubCategory/edit/74" target="_blank"&gt;Paniers de la mer&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/724" target="_blank"&gt;#724 Panier composé&lt;/a&gt; (246 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#46 &lt;a href="/db/TxpSubCategory/edit/46" target="_blank"&gt;Poissons fumés&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/324" target="_blank"&gt;#324 Poisson de mer fumé&lt;/a&gt; (208 produits),
+						 &lt;a href="/db/TxpProduct/edit/328" target="_blank"&gt;#328 Poisson d’eau douce fumé&lt;/a&gt; (127 produits),
+					&lt;/p&gt;
+				&lt;/td&gt;
+			&lt;/tr&gt;
+			&lt;tr&gt;
+				&lt;th&gt;
+					&lt;h4&gt;#8&lt;/h4&gt;
+					&lt;img src="/img/taxo/crem.png" style="width:120px;"/&gt;
+					&lt;br/&gt;
+					&lt;h4&gt;&lt;a href="/db/TxpCategory/edit/8" target="_blank"&gt;Crèmerie&lt;/a&gt;&lt;/h4&gt;
+				&lt;/th&gt;
+				&lt;td&gt;
+					&lt;p&gt;
+						&lt;b&gt;#69 &lt;a href="/db/TxpSubCategory/edit/69" target="_blank"&gt;Fromages de vache&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/83" target="_blank"&gt;#83 Fromage (vache)&lt;/a&gt; (15257 produits),
+						 &lt;a href="/db/TxpProduct/edit/689" target="_blank"&gt;#689 Pâtes molles à croûte fleurie&lt;/a&gt; (9 produits),
+						 &lt;a href="/db/TxpProduct/edit/690" target="_blank"&gt;#690 Pâtes pressées cuites&lt;/a&gt; (4 produits),
+						 &lt;a href="/db/TxpProduct/edit/691" target="_blank"&gt;#691 Pâtes pressées non-cuites&lt;/a&gt; (24 produits),
+						 &lt;a href="/db/TxpProduct/edit/692" target="_blank"&gt;#692 Pâtes molles à croûte lavée&lt;/a&gt; (14 produits),
+						 &lt;a href="/db/TxpProduct/edit/693" target="_blank"&gt;#693 Pâtes persillées&lt;/a&gt; (16 produits),
+						 &lt;a href="/db/TxpProduct/edit/694" target="_blank"&gt;#694 Fromages frais&lt;/a&gt; (158 produits),
+						 &lt;a href="/db/TxpProduct/edit/695" target="_blank"&gt;#695 Assortiment de fromages&lt;/a&gt; (36 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#70 &lt;a href="/db/TxpSubCategory/edit/70" target="_blank"&gt;Fromages de chèvre&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/664" target="_blank"&gt;#664 Fromage (chèvre)&lt;/a&gt; (14513 produits),
+						 &lt;a href="/db/TxpProduct/edit/696" target="_blank"&gt;#696 Fromages frais&lt;/a&gt; (171 produits),
+						 &lt;a href="/db/TxpProduct/edit/697" target="_blank"&gt;#697 Fromages à pâte molle et croûte naturelle&lt;/a&gt; (3 produits),
+						 &lt;a href="/db/TxpProduct/edit/698" target="_blank"&gt;#698 Fromage à pâte molle et croûte fleurie&lt;/a&gt; (22 produits),
+						 &lt;a href="/db/TxpProduct/edit/699" target="_blank"&gt;#699 Fromages à pâte pressée&lt;/a&gt; (14 produits),
+						 &lt;a href="/db/TxpProduct/edit/700" target="_blank"&gt;#700 Assortiment de fromages&lt;/a&gt; (0 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#71 &lt;a href="/db/TxpSubCategory/edit/71" target="_blank"&gt;Fromages de brebis&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/426" target="_blank"&gt;#426 Fromage (brebis)&lt;/a&gt; (3258 produits),
+						 &lt;a href="/db/TxpProduct/edit/701" target="_blank"&gt;#701 Fromages frais&lt;/a&gt; (44 produits),
+						 &lt;a href="/db/TxpProduct/edit/702" target="_blank"&gt;#702 Fromages à pâte molle et croûte naturelle&lt;/a&gt; (7 produits),
+						 &lt;a href="/db/TxpProduct/edit/703" target="_blank"&gt;#703 Fromages à pâte molle et croûte fleurie&lt;/a&gt; (8 produits),
+						 &lt;a href="/db/TxpProduct/edit/704" target="_blank"&gt;#704 Fromages à pâte pressée&lt;/a&gt; (64 produits),
+						 &lt;a href="/db/TxpProduct/edit/705" target="_blank"&gt;#705 Assortiment de fromages&lt;/a&gt; (3 produits),
+						 &lt;a href="/db/TxpProduct/edit/746" target="_blank"&gt;#746 Pâtes persillées&lt;/a&gt; (3 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#29 &lt;a href="/db/TxpSubCategory/edit/29" target="_blank"&gt;Desserts lactés et fromages frais&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/103" target="_blank"&gt;#103 Faisselle&lt;/a&gt; (1184 produits),
+						 &lt;a href="/db/TxpProduct/edit/104" target="_blank"&gt;#104 Fromage blanc&lt;/a&gt; (2268 produits),
+						 &lt;a href="/db/TxpProduct/edit/105" target="_blank"&gt;#105 Lait fermenté&lt;/a&gt; (117 produits),
+						 &lt;a href="/db/TxpProduct/edit/136" target="_blank"&gt;#136 Yaourt&lt;/a&gt; (8456 produits),
+						 &lt;a href="/db/TxpProduct/edit/706" target="_blank"&gt;#706 Crème dessert&lt;/a&gt; (375 produits),
+						 &lt;a href="/db/TxpProduct/edit/710" target="_blank"&gt;#710 Faisselle de vache&lt;/a&gt; (21 produits),
+						 &lt;a href="/db/TxpProduct/edit/711" target="_blank"&gt;#711 Faisselle de chèvre&lt;/a&gt; (20 produits),
+						 &lt;a href="/db/TxpProduct/edit/712" target="_blank"&gt;#712 Faisselle de brebis&lt;/a&gt; (6 produits),
+						 &lt;a href="/db/TxpProduct/edit/713" target="_blank"&gt;#713 Fromage blanc de vache&lt;/a&gt; (50 produits),
+						 &lt;a href="/db/TxpProduct/edit/714" target="_blank"&gt;#714 Fromage blanc de chèvre&lt;/a&gt; (13 produits),
+						 &lt;a href="/db/TxpProduct/edit/715" target="_blank"&gt;#715 Fromage blanc de brebis&lt;/a&gt; (13 produits),
+						 &lt;a href="/db/TxpProduct/edit/716" target="_blank"&gt;#716 Yaourt de vache&lt;/a&gt; (225 produits),
+						 &lt;a href="/db/TxpProduct/edit/717" target="_blank"&gt;#717 Yaourt de chèvre&lt;/a&gt; (66 produits),
+						 &lt;a href="/db/TxpProduct/edit/718" target="_blank"&gt;#718 Yaourt de brebis&lt;/a&gt; (171 produits),
+						 &lt;a href="/db/TxpProduct/edit/719" target="_blank"&gt;#719 Crème dessert de vache&lt;/a&gt; (66 produits),
+						 &lt;a href="/db/TxpProduct/edit/720" target="_blank"&gt;#720 Crème dessert de chèvre&lt;/a&gt; (127 produits),
+						 &lt;a href="/db/TxpProduct/edit/721" target="_blank"&gt;#721 Crème dessert de brebis&lt;/a&gt; (84 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#10 &lt;a href="/db/TxpSubCategory/edit/10" target="_blank"&gt;Beurre et crème fraîche&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/16" target="_blank"&gt;#16 Beurre&lt;/a&gt; (894 produits),
+						 &lt;a href="/db/TxpProduct/edit/425" target="_blank"&gt;#425 Crème fraîche&lt;/a&gt; (676 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#54 &lt;a href="/db/TxpSubCategory/edit/54" target="_blank"&gt;Lait&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/399" target="_blank"&gt;#399 Lait de vache&lt;/a&gt; (983 produits),
+						 &lt;a href="/db/TxpProduct/edit/400" target="_blank"&gt;#400 Lait d'ânesse&lt;/a&gt; (30 produits),
+						 &lt;a href="/db/TxpProduct/edit/402" target="_blank"&gt;#402 Lait de jument&lt;/a&gt; (27 produits),
+						 &lt;a href="/db/TxpProduct/edit/665" target="_blank"&gt;#665 Lait de chèvre&lt;/a&gt; (266 produits),
+						 &lt;a href="/db/TxpProduct/edit/726" target="_blank"&gt;#726 laits végétaux&lt;/a&gt; (16 produits),
+						 &lt;a href="/db/TxpProduct/edit/747" target="_blank"&gt;#747 Lait de brebis&lt;/a&gt; (11 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#19 &lt;a href="/db/TxpSubCategory/edit/19" target="_blank"&gt;Glaces &amp;amp; Sorbets&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/54" target="_blank"&gt;#54 Glace&lt;/a&gt; (3877 produits),
+						 &lt;a href="/db/TxpProduct/edit/106" target="_blank"&gt;#106 Dessert glacé&lt;/a&gt; (1684 produits),
+						 &lt;a href="/db/TxpProduct/edit/165" target="_blank"&gt;#165 Glace individuelle&lt;/a&gt; (168 produits),
+						 &lt;a href="/db/TxpProduct/edit/332" target="_blank"&gt;#332 Sorbet&lt;/a&gt; (2019 produits),
+						 &lt;a href="/db/TxpProduct/edit/708" target="_blank"&gt;#708 Glace au lait de vache&lt;/a&gt; (107 produits),
+						 &lt;a href="/db/TxpProduct/edit/709" target="_blank"&gt;#709 Glace au lait de chèvre&lt;/a&gt; (142 produits),
+						 &lt;a href="/db/TxpProduct/edit/748" target="_blank"&gt;#748 Glace au lait de brebis&lt;/a&gt; (0 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#50 &lt;a href="/db/TxpSubCategory/edit/50" target="_blank"&gt;Œufs&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/335" target="_blank"&gt;#335 Oeufs&lt;/a&gt; (3979 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#91 &lt;a href="/db/TxpSubCategory/edit/91" target="_blank"&gt;Paniers composés et fromages mixtes&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/666" target="_blank"&gt;#666 Assortiment de fromages&lt;/a&gt; (710 produits),
+						 &lt;a href="/db/TxpProduct/edit/798" target="_blank"&gt;#798 paniers composés&lt;/a&gt; (22 produits),
+						 &lt;a href="/db/TxpProduct/edit/800" target="_blank"&gt;#800 Fromages mixtes&lt;/a&gt; (1 produits),
+					&lt;/p&gt;
+				&lt;/td&gt;
+			&lt;/tr&gt;
+			&lt;tr&gt;
+				&lt;th&gt;
+					&lt;h4&gt;#7&lt;/h4&gt;
+					&lt;img src="/img/taxo/boulangerie.png" style="width:120px;"/&gt;
+					&lt;br/&gt;
+					&lt;h4&gt;&lt;a href="/db/TxpCategory/edit/7" target="_blank"&gt;Boulangerie et pâtisserie&lt;/a&gt;&lt;/h4&gt;
+				&lt;/th&gt;
+				&lt;td&gt;
+					&lt;p&gt;
+						&lt;b&gt;#9 &lt;a href="/db/TxpSubCategory/edit/9" target="_blank"&gt;Tartes, gâteaux et biscuits&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/14" target="_blank"&gt;#14 Gâteaux&lt;/a&gt; (2043 produits),
+						 &lt;a href="/db/TxpProduct/edit/771" target="_blank"&gt;#771 Tartes&lt;/a&gt; (1826 produits),
+						 &lt;a href="/db/TxpProduct/edit/773" target="_blank"&gt;#773 Biscuits&lt;/a&gt; (7045 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#13 &lt;a href="/db/TxpSubCategory/edit/13" target="_blank"&gt;Viennoiseries&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/22" target="_blank"&gt;#22 Brioche&lt;/a&gt; (2423 produits),
+						 &lt;a href="/db/TxpProduct/edit/149" target="_blank"&gt;#149 Viennoiserie&lt;/a&gt; (714 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#31 &lt;a href="/db/TxpSubCategory/edit/31" target="_blank"&gt;Galettes, Crêpes et Pizzas&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/114" target="_blank"&gt;#114 Galette de blé noir&lt;/a&gt; (114 produits),
+						 &lt;a href="/db/TxpProduct/edit/147" target="_blank"&gt;#147 Crêpe&lt;/a&gt; (142 produits),
+						 &lt;a href="/db/TxpProduct/edit/674" target="_blank"&gt;#674 Galette Céréales&lt;/a&gt; (1557 produits),
+						 &lt;a href="/db/TxpProduct/edit/723" target="_blank"&gt;#723 Pizzas&lt;/a&gt; (101 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#32 &lt;a href="/db/TxpSubCategory/edit/32" target="_blank"&gt;Pains&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/118" target="_blank"&gt;#118 Pain lin pavot&lt;/a&gt; (87 produits),
+						 &lt;a href="/db/TxpProduct/edit/119" target="_blank"&gt;#119 Pain multigraines&lt;/a&gt; (1970 produits),
+						 &lt;a href="/db/TxpProduct/edit/120" target="_blank"&gt;#120 Pain nature&lt;/a&gt; (1362 produits),
+						 &lt;a href="/db/TxpProduct/edit/121" target="_blank"&gt;#121 Pain sésame&lt;/a&gt; (288 produits),
+						 &lt;a href="/db/TxpProduct/edit/123" target="_blank"&gt;#123 Pain au noix&lt;/a&gt; (718 produits),
+						 &lt;a href="/db/TxpProduct/edit/124" target="_blank"&gt;#124 Pain aux graines de courge&lt;/a&gt; (249 produits),
+						 &lt;a href="/db/TxpProduct/edit/125" target="_blank"&gt;#125 Pain aux raisins&lt;/a&gt; (484 produits),
+						 &lt;a href="/db/TxpProduct/edit/127" target="_blank"&gt;#127 Pain complet&lt;/a&gt; (1461 produits),
+						 &lt;a href="/db/TxpProduct/edit/128" target="_blank"&gt;#128 Pain de campagne&lt;/a&gt; (1084 produits),
+						 &lt;a href="/db/TxpProduct/edit/129" target="_blank"&gt;#129 Pain demi-complet&lt;/a&gt; (2029 produits),
+						 &lt;a href="/db/TxpProduct/edit/148" target="_blank"&gt;#148 Tous pains&lt;/a&gt; (7548 produits),
+						 &lt;a href="/db/TxpProduct/edit/442" target="_blank"&gt;#442 Pain tournesol&lt;/a&gt; (294 produits),
+						 &lt;a href="/db/TxpProduct/edit/443" target="_blank"&gt;#443 Pain à l'engrain&lt;/a&gt; (658 produits),
+						 &lt;a href="/db/TxpProduct/edit/444" target="_blank"&gt;#444 Pain à l'épeautre&lt;/a&gt; (739 produits),
+						 &lt;a href="/db/TxpProduct/edit/672" target="_blank"&gt;#672 Biscottes&lt;/a&gt; (423 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#73 &lt;a href="/db/TxpSubCategory/edit/73" target="_blank"&gt;Pâtes à cuisiner&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/15" target="_blank"&gt;#15 Pâte à tarte&lt;/a&gt; (263 produits),
+						 &lt;a href="/db/TxpProduct/edit/707" target="_blank"&gt;#707 Pâte à pizza&lt;/a&gt; (13 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#98 &lt;a href="/db/TxpSubCategory/edit/98" target="_blank"&gt;Farines&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/226" target="_blank"&gt;#226 Farine&lt;/a&gt; (14302 produits),
+						 &lt;a href="/db/TxpProduct/edit/781" target="_blank"&gt;#781 Farine complète&lt;/a&gt; (85 produits),
+						 &lt;a href="/db/TxpProduct/edit/782" target="_blank"&gt;#782 Farine semi-complète&lt;/a&gt; (287 produits),
+						 &lt;a href="/db/TxpProduct/edit/783" target="_blank"&gt;#783 Farine blanche&lt;/a&gt; (56 produits),
+						 &lt;a href="/db/TxpProduct/edit/784" target="_blank"&gt;#784 Farine intégrale&lt;/a&gt; (26 produits),
+					&lt;/p&gt;
+				&lt;/td&gt;
+			&lt;/tr&gt;
+			&lt;tr&gt;
+				&lt;th&gt;
+					&lt;h4&gt;#14&lt;/h4&gt;
+					&lt;img src="/img/taxo/epic.png" style="width:120px;"/&gt;
+					&lt;br/&gt;
+					&lt;h4&gt;&lt;a href="/db/TxpCategory/edit/14" target="_blank"&gt;Épicerie&lt;/a&gt;&lt;/h4&gt;
+				&lt;/th&gt;
+				&lt;td&gt;
+					&lt;p&gt;
+						&lt;b&gt;#4 &lt;a href="/db/TxpSubCategory/edit/4" target="_blank"&gt;Petit-déjeuner et plats cuisinés&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/66" target="_blank"&gt;#66 Plat cuisiné&lt;/a&gt; (5685 produits),
+						 &lt;a href="/db/TxpProduct/edit/139" target="_blank"&gt;#139 Dessert&lt;/a&gt; (2546 produits),
+						 &lt;a href="/db/TxpProduct/edit/673" target="_blank"&gt;#673 Céréales petit-déj.&lt;/a&gt; (4077 produits),
+						 &lt;a href="/db/TxpProduct/edit/681" target="_blank"&gt;#681 Pots bébé&lt;/a&gt; (1270 produits),
+						 &lt;a href="/db/TxpProduct/edit/795" target="_blank"&gt;#795 Entrées&lt;/a&gt; (50 produits),
+						 &lt;a href="/db/TxpProduct/edit/796" target="_blank"&gt;#796 Plats&lt;/a&gt; (9 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#30 &lt;a href="/db/TxpSubCategory/edit/30" target="_blank"&gt;Soupes et Conserves&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/107" target="_blank"&gt;#107 Conserves de fruits&lt;/a&gt; (103 produits),
+						 &lt;a href="/db/TxpProduct/edit/428" target="_blank"&gt;#428 Soupe&lt;/a&gt; (3081 produits),
+						 &lt;a href="/db/TxpProduct/edit/431" target="_blank"&gt;#431 Conserves de légumes&lt;/a&gt; (3787 produits),
+						 &lt;a href="/db/TxpProduct/edit/793" target="_blank"&gt;#793 Conserves de viande&lt;/a&gt; (1933 produits),
+						 &lt;a href="/db/TxpProduct/edit/802" target="_blank"&gt;#802 Conserves lacto-fermentées&lt;/a&gt; (28 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#35 &lt;a href="/db/TxpSubCategory/edit/35" target="_blank"&gt;Pâtes et riz&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/475" target="_blank"&gt;#475 Pâtes&lt;/a&gt; (31590 produits),
+						 &lt;a href="/db/TxpProduct/edit/794" target="_blank"&gt;#794 Riz&lt;/a&gt; (8836 produits),
+					&lt;/p&gt;
+					&lt;p&gt;
+						&lt;b&gt;#38 &lt;a href="/db/TxpSubCategory/edit/38" target="_blank"&gt;Condiments et sauces&lt;/a&gt;&lt;/b&gt;
+						&lt;br/&gt;
+						 &lt;a href="/db/TxpProduct/edit/161" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i &lt; j.length</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> i++) {</t>
   </si>
 </sst>
 </file>
@@ -2082,58 +2706,57 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D382"/>
+  <dimension ref="A2:D453"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D388" activeCellId="0" sqref="D388"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A504" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A387" activeCellId="0" sqref="A387:A525"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="35.05"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="0" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="0" t="s">
@@ -2141,7 +2764,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="0" t="s">
@@ -2149,7 +2772,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="0" t="s">
@@ -2157,76 +2780,76 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="2" t="s">
+      <c r="B7" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="0" t="s">
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="0" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C12" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C14" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="1" t="s">
+      <c r="D15" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="0" t="s">
@@ -2234,7 +2857,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -2242,7 +2865,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D18" s="0" t="s">
@@ -2250,12 +2873,12 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="0" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="0" t="s">
@@ -2263,7 +2886,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="0" t="s">
@@ -2271,7 +2894,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="0" t="s">
@@ -2279,7 +2902,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D23" s="0" t="s">
@@ -2287,7 +2910,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="0" t="s">
@@ -2295,7 +2918,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D25" s="0" t="s">
@@ -2303,7 +2926,7 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D26" s="0" t="s">
@@ -2311,12 +2934,12 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="0" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D28" s="0" t="s">
@@ -2324,7 +2947,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D29" s="0" t="s">
@@ -2332,7 +2955,7 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D30" s="0" t="s">
@@ -2340,7 +2963,7 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D31" s="0" t="s">
@@ -2348,12 +2971,12 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="0" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D33" s="0" t="s">
@@ -2361,7 +2984,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D34" s="0" t="s">
@@ -2369,7 +2992,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="1" t="s">
         <v>60</v>
       </c>
       <c r="D35" s="0" t="s">
@@ -2377,7 +3000,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="1" t="s">
         <v>62</v>
       </c>
       <c r="D36" s="0" t="s">
@@ -2385,7 +3008,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="1" t="s">
         <v>64</v>
       </c>
       <c r="D37" s="0" t="s">
@@ -2393,7 +3016,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="1" t="s">
         <v>66</v>
       </c>
       <c r="D38" s="0" t="s">
@@ -2401,7 +3024,7 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="1" t="s">
         <v>68</v>
       </c>
       <c r="D39" s="0" t="s">
@@ -2409,7 +3032,7 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D40" s="0" t="s">
@@ -2417,25 +3040,25 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="1" t="s">
         <v>71</v>
       </c>
       <c r="D41" s="0" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="0" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="1" t="s">
         <v>75</v>
       </c>
       <c r="D44" s="0" t="s">
@@ -2443,12 +3066,12 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="0" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D46" s="0" t="s">
@@ -2456,7 +3079,7 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D47" s="0" t="s">
@@ -2464,7 +3087,7 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>82</v>
       </c>
       <c r="D48" s="0" t="s">
@@ -2472,7 +3095,7 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>84</v>
       </c>
       <c r="D49" s="0" t="s">
@@ -2480,7 +3103,7 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="1" t="s">
         <v>86</v>
       </c>
       <c r="D50" s="0" t="s">
@@ -2488,7 +3111,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D51" s="0" t="s">
@@ -2496,7 +3119,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>90</v>
       </c>
       <c r="D52" s="0" t="s">
@@ -2504,7 +3127,7 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="1" t="s">
         <v>92</v>
       </c>
       <c r="D53" s="0" t="s">
@@ -2512,7 +3135,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>94</v>
       </c>
       <c r="D54" s="0" t="s">
@@ -2520,7 +3143,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>96</v>
       </c>
       <c r="D55" s="0" t="s">
@@ -2528,7 +3151,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>98</v>
       </c>
       <c r="D56" s="0" t="s">
@@ -2536,7 +3159,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C57" s="2" t="s">
+      <c r="C57" s="1" t="s">
         <v>100</v>
       </c>
       <c r="D57" s="0" t="s">
@@ -2544,7 +3167,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D58" s="0" t="s">
@@ -2552,12 +3175,12 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="0" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C60" s="2" t="s">
+      <c r="C60" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D60" s="0" t="s">
@@ -2565,7 +3188,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C61" s="2" t="s">
+      <c r="C61" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D61" s="0" t="s">
@@ -2573,12 +3196,12 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="1" t="s">
+      <c r="B62" s="0" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="2" t="s">
+      <c r="C63" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D63" s="0" t="s">
@@ -2586,12 +3209,12 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="0" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C65" s="2" t="s">
+      <c r="C65" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D65" s="0" t="s">
@@ -2599,7 +3222,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C66" s="2" t="s">
+      <c r="C66" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D66" s="0" t="s">
@@ -2607,12 +3230,12 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="0" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="1" t="s">
         <v>118</v>
       </c>
       <c r="D68" s="0" t="s">
@@ -2620,12 +3243,12 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="0" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="1" t="s">
         <v>121</v>
       </c>
       <c r="D70" s="0" t="s">
@@ -2633,7 +3256,7 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C71" s="2" t="s">
+      <c r="C71" s="1" t="s">
         <v>123</v>
       </c>
       <c r="D71" s="0" t="s">
@@ -2641,7 +3264,7 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C72" s="2" t="s">
+      <c r="C72" s="1" t="s">
         <v>125</v>
       </c>
       <c r="D72" s="0" t="s">
@@ -2649,12 +3272,12 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="0" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="1" t="s">
         <v>128</v>
       </c>
       <c r="D74" s="0" t="s">
@@ -2662,12 +3285,12 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="0" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C76" s="2" t="s">
+      <c r="C76" s="1" t="s">
         <v>130</v>
       </c>
       <c r="D76" s="0" t="s">
@@ -2675,7 +3298,7 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="1" t="s">
         <v>132</v>
       </c>
       <c r="D77" s="0" t="s">
@@ -2683,7 +3306,7 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="1" t="s">
         <v>134</v>
       </c>
       <c r="D78" s="0" t="s">
@@ -2691,7 +3314,7 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="1" t="s">
         <v>136</v>
       </c>
       <c r="D79" s="0" t="s">
@@ -2699,7 +3322,7 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C80" s="2" t="s">
+      <c r="C80" s="1" t="s">
         <v>138</v>
       </c>
       <c r="D80" s="0" t="s">
@@ -2707,12 +3330,12 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="1" t="s">
+      <c r="B81" s="0" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="2" t="s">
+      <c r="C82" s="1" t="s">
         <v>141</v>
       </c>
       <c r="D82" s="0" t="s">
@@ -2720,7 +3343,7 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="2" t="s">
+      <c r="C83" s="1" t="s">
         <v>143</v>
       </c>
       <c r="D83" s="0" t="s">
@@ -2728,7 +3351,7 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="2" t="s">
+      <c r="C84" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D84" s="0" t="s">
@@ -2736,12 +3359,12 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="1" t="s">
+      <c r="B85" s="0" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="2" t="s">
+      <c r="C86" s="1" t="s">
         <v>148</v>
       </c>
       <c r="D86" s="0" t="s">
@@ -2749,7 +3372,7 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="2" t="s">
+      <c r="C87" s="1" t="s">
         <v>150</v>
       </c>
       <c r="D87" s="0" t="s">
@@ -2757,7 +3380,7 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="2" t="s">
+      <c r="C88" s="1" t="s">
         <v>152</v>
       </c>
       <c r="D88" s="0" t="s">
@@ -2765,7 +3388,7 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="2" t="s">
+      <c r="C89" s="1" t="s">
         <v>154</v>
       </c>
       <c r="D89" s="0" t="s">
@@ -2773,12 +3396,12 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="1" t="s">
+      <c r="B90" s="0" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="2" t="s">
+      <c r="C91" s="1" t="s">
         <v>157</v>
       </c>
       <c r="D91" s="0" t="s">
@@ -2786,7 +3409,7 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="2" t="s">
+      <c r="C92" s="1" t="s">
         <v>159</v>
       </c>
       <c r="D92" s="0" t="s">
@@ -2794,7 +3417,7 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="1" t="s">
         <v>161</v>
       </c>
       <c r="D93" s="0" t="s">
@@ -2802,25 +3425,25 @@
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="2" t="s">
+      <c r="C94" s="1" t="s">
         <v>163</v>
       </c>
       <c r="D94" s="0" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="1" t="s">
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="1" t="s">
+      <c r="B96" s="0" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="1" t="s">
         <v>166</v>
       </c>
       <c r="D97" s="0" t="s">
@@ -2828,7 +3451,7 @@
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="2" t="s">
+      <c r="C98" s="1" t="s">
         <v>168</v>
       </c>
       <c r="D98" s="0" t="s">
@@ -2836,20 +3459,20 @@
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="1" t="s">
         <v>170</v>
       </c>
       <c r="D99" s="0" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="1" t="s">
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="0" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="2" t="s">
+      <c r="C101" s="1" t="s">
         <v>173</v>
       </c>
       <c r="D101" s="0" t="s">
@@ -2857,7 +3480,7 @@
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="2" t="s">
+      <c r="C102" s="1" t="s">
         <v>175</v>
       </c>
       <c r="D102" s="0" t="s">
@@ -2865,7 +3488,7 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="2" t="s">
+      <c r="C103" s="1" t="s">
         <v>177</v>
       </c>
       <c r="D103" s="0" t="s">
@@ -2873,12 +3496,12 @@
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="0" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="2" t="s">
+      <c r="C105" s="1" t="s">
         <v>180</v>
       </c>
       <c r="D105" s="0" t="s">
@@ -2886,12 +3509,12 @@
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="1" t="s">
+      <c r="B106" s="0" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="2" t="s">
+      <c r="C107" s="1" t="s">
         <v>183</v>
       </c>
       <c r="D107" s="0" t="s">
@@ -2899,12 +3522,12 @@
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="1" t="s">
+      <c r="B108" s="0" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C109" s="2" t="s">
+      <c r="C109" s="1" t="s">
         <v>185</v>
       </c>
       <c r="D109" s="0" t="s">
@@ -2912,12 +3535,12 @@
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="1" t="s">
+      <c r="B110" s="0" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="2" t="s">
+      <c r="C111" s="1" t="s">
         <v>188</v>
       </c>
       <c r="D111" s="0" t="s">
@@ -2925,7 +3548,7 @@
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="2" t="s">
+      <c r="C112" s="1" t="s">
         <v>190</v>
       </c>
       <c r="D112" s="0" t="s">
@@ -2933,17 +3556,17 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="0" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="1" t="s">
+      <c r="B114" s="0" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="2" t="s">
+      <c r="C115" s="1" t="s">
         <v>194</v>
       </c>
       <c r="D115" s="0" t="s">
@@ -2951,7 +3574,7 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="2" t="s">
+      <c r="C116" s="1" t="s">
         <v>196</v>
       </c>
       <c r="D116" s="0" t="s">
@@ -2959,7 +3582,7 @@
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="2" t="s">
+      <c r="C117" s="1" t="s">
         <v>198</v>
       </c>
       <c r="D117" s="0" t="s">
@@ -2967,7 +3590,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="2" t="s">
+      <c r="C118" s="1" t="s">
         <v>200</v>
       </c>
       <c r="D118" s="0" t="s">
@@ -2975,7 +3598,7 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="2" t="s">
+      <c r="C119" s="1" t="s">
         <v>202</v>
       </c>
       <c r="D119" s="0" t="s">
@@ -2983,7 +3606,7 @@
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="2" t="s">
+      <c r="C120" s="1" t="s">
         <v>204</v>
       </c>
       <c r="D120" s="0" t="s">
@@ -2991,7 +3614,7 @@
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="2" t="s">
+      <c r="C121" s="1" t="s">
         <v>206</v>
       </c>
       <c r="D121" s="0" t="s">
@@ -2999,7 +3622,7 @@
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="2" t="s">
+      <c r="C122" s="1" t="s">
         <v>208</v>
       </c>
       <c r="D122" s="0" t="s">
@@ -3007,12 +3630,12 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="0" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C124" s="2" t="s">
+      <c r="C124" s="1" t="s">
         <v>211</v>
       </c>
       <c r="D124" s="0" t="s">
@@ -3020,7 +3643,7 @@
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C125" s="2" t="s">
+      <c r="C125" s="1" t="s">
         <v>213</v>
       </c>
       <c r="D125" s="0" t="s">
@@ -3028,7 +3651,7 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C126" s="2" t="s">
+      <c r="C126" s="1" t="s">
         <v>214</v>
       </c>
       <c r="D126" s="0" t="s">
@@ -3036,7 +3659,7 @@
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C127" s="2" t="s">
+      <c r="C127" s="1" t="s">
         <v>216</v>
       </c>
       <c r="D127" s="0" t="s">
@@ -3044,7 +3667,7 @@
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C128" s="2" t="s">
+      <c r="C128" s="1" t="s">
         <v>218</v>
       </c>
       <c r="D128" s="0" t="s">
@@ -3052,7 +3675,7 @@
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C129" s="2" t="s">
+      <c r="C129" s="1" t="s">
         <v>220</v>
       </c>
       <c r="D129" s="0" t="s">
@@ -3060,12 +3683,12 @@
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B130" s="1" t="s">
+      <c r="B130" s="0" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="1" t="s">
         <v>222</v>
       </c>
       <c r="D131" s="0" t="s">
@@ -3073,7 +3696,7 @@
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C132" s="2" t="s">
+      <c r="C132" s="1" t="s">
         <v>224</v>
       </c>
       <c r="D132" s="0" t="s">
@@ -3081,7 +3704,7 @@
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C133" s="2" t="s">
+      <c r="C133" s="1" t="s">
         <v>225</v>
       </c>
       <c r="D133" s="0" t="s">
@@ -3089,7 +3712,7 @@
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C134" s="2" t="s">
+      <c r="C134" s="1" t="s">
         <v>226</v>
       </c>
       <c r="D134" s="0" t="s">
@@ -3097,7 +3720,7 @@
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C135" s="2" t="s">
+      <c r="C135" s="1" t="s">
         <v>228</v>
       </c>
       <c r="D135" s="0" t="s">
@@ -3105,7 +3728,7 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="1" t="s">
         <v>229</v>
       </c>
       <c r="D136" s="0" t="s">
@@ -3113,20 +3736,20 @@
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C137" s="2" t="s">
+      <c r="C137" s="1" t="s">
         <v>230</v>
       </c>
       <c r="D137" s="0" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B138" s="1" t="s">
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B138" s="0" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="1" t="s">
         <v>232</v>
       </c>
       <c r="D139" s="0" t="s">
@@ -3134,7 +3757,7 @@
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C140" s="2" t="s">
+      <c r="C140" s="1" t="s">
         <v>234</v>
       </c>
       <c r="D140" s="0" t="s">
@@ -3142,7 +3765,7 @@
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C141" s="2" t="s">
+      <c r="C141" s="1" t="s">
         <v>236</v>
       </c>
       <c r="D141" s="0" t="s">
@@ -3150,7 +3773,7 @@
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="1" t="s">
         <v>238</v>
       </c>
       <c r="D142" s="0" t="s">
@@ -3158,7 +3781,7 @@
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C143" s="2" t="s">
+      <c r="C143" s="1" t="s">
         <v>240</v>
       </c>
       <c r="D143" s="0" t="s">
@@ -3166,7 +3789,7 @@
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C144" s="2" t="s">
+      <c r="C144" s="1" t="s">
         <v>242</v>
       </c>
       <c r="D144" s="0" t="s">
@@ -3174,7 +3797,7 @@
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C145" s="2" t="s">
+      <c r="C145" s="1" t="s">
         <v>244</v>
       </c>
       <c r="D145" s="0" t="s">
@@ -3182,7 +3805,7 @@
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C146" s="2" t="s">
+      <c r="C146" s="1" t="s">
         <v>246</v>
       </c>
       <c r="D146" s="0" t="s">
@@ -3190,7 +3813,7 @@
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C147" s="2" t="s">
+      <c r="C147" s="1" t="s">
         <v>248</v>
       </c>
       <c r="D147" s="0" t="s">
@@ -3198,7 +3821,7 @@
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C148" s="2" t="s">
+      <c r="C148" s="1" t="s">
         <v>250</v>
       </c>
       <c r="D148" s="0" t="s">
@@ -3206,7 +3829,7 @@
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C149" s="2" t="s">
+      <c r="C149" s="1" t="s">
         <v>252</v>
       </c>
       <c r="D149" s="0" t="s">
@@ -3214,7 +3837,7 @@
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C150" s="2" t="s">
+      <c r="C150" s="1" t="s">
         <v>254</v>
       </c>
       <c r="D150" s="0" t="s">
@@ -3222,7 +3845,7 @@
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C151" s="2" t="s">
+      <c r="C151" s="1" t="s">
         <v>256</v>
       </c>
       <c r="D151" s="0" t="s">
@@ -3230,7 +3853,7 @@
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C152" s="2" t="s">
+      <c r="C152" s="1" t="s">
         <v>258</v>
       </c>
       <c r="D152" s="0" t="s">
@@ -3238,7 +3861,7 @@
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C153" s="2" t="s">
+      <c r="C153" s="1" t="s">
         <v>260</v>
       </c>
       <c r="D153" s="0" t="s">
@@ -3246,7 +3869,7 @@
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C154" s="2" t="s">
+      <c r="C154" s="1" t="s">
         <v>262</v>
       </c>
       <c r="D154" s="0" t="s">
@@ -3254,7 +3877,7 @@
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C155" s="2" t="s">
+      <c r="C155" s="1" t="s">
         <v>264</v>
       </c>
       <c r="D155" s="0" t="s">
@@ -3262,12 +3885,12 @@
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B156" s="1" t="s">
+      <c r="B156" s="0" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C157" s="2" t="s">
+      <c r="C157" s="1" t="s">
         <v>267</v>
       </c>
       <c r="D157" s="0" t="s">
@@ -3275,7 +3898,7 @@
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C158" s="2" t="s">
+      <c r="C158" s="1" t="s">
         <v>269</v>
       </c>
       <c r="D158" s="0" t="s">
@@ -3283,12 +3906,12 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B159" s="1" t="s">
+      <c r="B159" s="0" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C160" s="2" t="s">
+      <c r="C160" s="1" t="s">
         <v>272</v>
       </c>
       <c r="D160" s="0" t="s">
@@ -3296,7 +3919,7 @@
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C161" s="2" t="s">
+      <c r="C161" s="1" t="s">
         <v>274</v>
       </c>
       <c r="D161" s="0" t="s">
@@ -3304,7 +3927,7 @@
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C162" s="2" t="s">
+      <c r="C162" s="1" t="s">
         <v>276</v>
       </c>
       <c r="D162" s="0" t="s">
@@ -3312,7 +3935,7 @@
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C163" s="2" t="s">
+      <c r="C163" s="1" t="s">
         <v>278</v>
       </c>
       <c r="D163" s="0" t="s">
@@ -3320,7 +3943,7 @@
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C164" s="2" t="s">
+      <c r="C164" s="1" t="s">
         <v>280</v>
       </c>
       <c r="D164" s="0" t="s">
@@ -3328,7 +3951,7 @@
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C165" s="2" t="s">
+      <c r="C165" s="1" t="s">
         <v>282</v>
       </c>
       <c r="D165" s="0" t="s">
@@ -3336,12 +3959,12 @@
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B166" s="1" t="s">
+      <c r="B166" s="0" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C167" s="2" t="s">
+      <c r="C167" s="1" t="s">
         <v>285</v>
       </c>
       <c r="D167" s="0" t="s">
@@ -3349,7 +3972,7 @@
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C168" s="2" t="s">
+      <c r="C168" s="1" t="s">
         <v>287</v>
       </c>
       <c r="D168" s="0" t="s">
@@ -3357,7 +3980,7 @@
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="1" t="s">
         <v>289</v>
       </c>
       <c r="D169" s="0" t="s">
@@ -3365,7 +3988,7 @@
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C170" s="2" t="s">
+      <c r="C170" s="1" t="s">
         <v>291</v>
       </c>
       <c r="D170" s="0" t="s">
@@ -3373,7 +3996,7 @@
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="1" t="s">
         <v>293</v>
       </c>
       <c r="D171" s="0" t="s">
@@ -3381,7 +4004,7 @@
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C172" s="2" t="s">
+      <c r="C172" s="1" t="s">
         <v>295</v>
       </c>
       <c r="D172" s="0" t="s">
@@ -3389,7 +4012,7 @@
       </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C173" s="2" t="s">
+      <c r="C173" s="1" t="s">
         <v>297</v>
       </c>
       <c r="D173" s="0" t="s">
@@ -3397,12 +4020,12 @@
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B174" s="1" t="s">
+      <c r="B174" s="0" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C175" s="2" t="s">
+      <c r="C175" s="1" t="s">
         <v>300</v>
       </c>
       <c r="D175" s="0" t="s">
@@ -3410,834 +4033,834 @@
       </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B176" s="1" t="s">
-        <v>24</v>
+      <c r="B176" s="0" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C177" s="2" t="s">
-        <v>302</v>
+      <c r="C177" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="D177" s="0" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C178" s="2" t="s">
-        <v>303</v>
+      <c r="C178" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="D178" s="0" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="180" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B180" s="1" t="s">
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C179" s="1" t="s">
         <v>306</v>
       </c>
+      <c r="D179" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C181" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="D181" s="0" t="s">
-        <v>308</v>
+      <c r="B181" s="0" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C182" s="2" t="s">
-        <v>309</v>
+      <c r="C182" s="1" t="s">
+        <v>310</v>
       </c>
       <c r="D182" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C183" s="2" t="s">
-        <v>311</v>
+      <c r="C183" s="1" t="s">
+        <v>312</v>
       </c>
       <c r="D183" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B184" s="1" t="s">
-        <v>313</v>
+      <c r="C184" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D184" s="0" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C185" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="D185" s="0" t="s">
-        <v>315</v>
+      <c r="B185" s="0" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C186" s="2" t="s">
-        <v>316</v>
+      <c r="C186" s="1" t="s">
+        <v>317</v>
       </c>
       <c r="D186" s="0" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B187" s="1" t="s">
         <v>318</v>
       </c>
     </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C187" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="D187" s="0" t="s">
+        <v>320</v>
+      </c>
+    </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C188" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="D188" s="0" t="s">
-        <v>320</v>
+      <c r="B188" s="0" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C189" s="2" t="s">
-        <v>321</v>
+      <c r="C189" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="D189" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C190" s="2" t="s">
-        <v>323</v>
+      <c r="C190" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="D190" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C191" s="2" t="s">
-        <v>325</v>
+      <c r="C191" s="1" t="s">
+        <v>326</v>
       </c>
       <c r="D191" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B192" s="1" t="s">
-        <v>327</v>
+      <c r="C192" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D192" s="0" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C193" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="D193" s="0" t="s">
-        <v>329</v>
+      <c r="B193" s="0" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C194" s="2" t="s">
-        <v>330</v>
+      <c r="C194" s="1" t="s">
+        <v>331</v>
       </c>
       <c r="D194" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C195" s="2" t="s">
-        <v>332</v>
+      <c r="C195" s="1" t="s">
+        <v>333</v>
       </c>
       <c r="D195" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C196" s="2" t="s">
-        <v>334</v>
+      <c r="C196" s="1" t="s">
+        <v>335</v>
       </c>
       <c r="D196" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C197" s="2" t="s">
-        <v>336</v>
+      <c r="C197" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="D197" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C198" s="2" t="s">
-        <v>338</v>
+      <c r="C198" s="1" t="s">
+        <v>339</v>
       </c>
       <c r="D198" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C199" s="2" t="s">
-        <v>340</v>
+      <c r="C199" s="1" t="s">
+        <v>341</v>
       </c>
       <c r="D199" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C200" s="2" t="s">
-        <v>342</v>
+      <c r="C200" s="1" t="s">
+        <v>343</v>
       </c>
       <c r="D200" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C201" s="2" t="s">
-        <v>344</v>
+      <c r="C201" s="1" t="s">
+        <v>345</v>
       </c>
       <c r="D201" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C202" s="2" t="s">
-        <v>346</v>
+      <c r="C202" s="1" t="s">
+        <v>347</v>
       </c>
       <c r="D202" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="2" t="s">
-        <v>348</v>
+      <c r="C203" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="D203" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="2" t="s">
-        <v>350</v>
+      <c r="C204" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="D204" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C205" s="2" t="s">
-        <v>352</v>
+      <c r="C205" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="D205" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="2" t="s">
-        <v>354</v>
+      <c r="C206" s="1" t="s">
+        <v>355</v>
       </c>
       <c r="D206" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="2" t="s">
-        <v>356</v>
+      <c r="C207" s="1" t="s">
+        <v>357</v>
       </c>
       <c r="D207" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B208" s="1" t="s">
-        <v>358</v>
+      <c r="C208" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D208" s="0" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C209" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="D209" s="0" t="s">
-        <v>360</v>
+      <c r="B209" s="0" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C210" s="2" t="s">
-        <v>361</v>
+      <c r="C210" s="1" t="s">
+        <v>362</v>
       </c>
       <c r="D210" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B211" s="1" t="s">
-        <v>363</v>
+      <c r="C211" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D211" s="0" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C212" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D212" s="0" t="s">
-        <v>365</v>
+      <c r="B212" s="0" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C213" s="2" t="s">
+      <c r="C213" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="D213" s="0" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C214" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="D214" s="0" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C215" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="D215" s="0" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C216" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="D216" s="0" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C217" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D217" s="0" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A218" s="0" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B219" s="0" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C220" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="D220" s="0" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C221" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="D221" s="0" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C222" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="D222" s="0" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C223" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="D223" s="0" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C224" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="D224" s="0" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C225" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D225" s="0" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B226" s="0" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C227" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D227" s="0" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C228" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C229" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="D229" s="0" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C230" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D230" s="0" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C231" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="D231" s="0" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B232" s="0" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C233" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D233" s="0" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C234" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D234" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B235" s="0" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C236" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D236" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C237" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D237" s="0" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B238" s="0" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C239" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D239" s="0" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B240" s="0" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C241" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D241" s="0" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C242" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="D242" s="0" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C243" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="D243" s="0" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B244" s="0" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C245" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D245" s="0" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C246" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D246" s="0" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C247" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D247" s="0" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B248" s="0" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C249" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D249" s="0" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C250" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="D250" s="0" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C251" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D251" s="0" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C252" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="D252" s="0" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B253" s="0" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C254" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="D254" s="0" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C255" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D255" s="0" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C256" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="D256" s="0" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C257" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D257" s="0" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C258" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="D258" s="0" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C259" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D259" s="0" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C260" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D260" s="0" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C261" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="D261" s="0" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C262" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="D262" s="0" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C263" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="D263" s="0" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C264" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="D264" s="0" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C265" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D265" s="0" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C266" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="D266" s="0" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C267" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="D267" s="0" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C268" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="D268" s="0" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C269" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D269" s="0" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C270" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D270" s="0" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B271" s="0" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C272" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="D272" s="0" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C273" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D273" s="0" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C274" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="D274" s="0" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C275" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="D275" s="0" t="s">
         <v>366</v>
       </c>
-      <c r="D213" s="0" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C214" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D214" s="0" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C215" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="D215" s="0" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C216" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="D216" s="0" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="1" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="218" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B218" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C219" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="D219" s="0" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C220" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="D220" s="0" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C221" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="D221" s="0" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C222" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="D222" s="0" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C223" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="D223" s="0" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C224" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="D224" s="0" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B225" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C226" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="D226" s="0" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C227" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="D227" s="0" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C228" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="D228" s="0" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C229" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="D229" s="0" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B230" s="1" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C231" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="D231" s="0" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C232" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="D232" s="0" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B233" s="1" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C234" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D234" s="0" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C235" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="D235" s="0" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B236" s="1" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C237" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="D237" s="0" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B238" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C239" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="D239" s="0" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C240" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="D240" s="0" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C241" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="D241" s="0" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B242" s="1" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C243" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D243" s="0" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C244" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D244" s="0" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C245" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="D245" s="0" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B246" s="1" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C247" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D247" s="0" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C248" s="2" t="s">
-        <v>426</v>
-      </c>
-      <c r="D248" s="0" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C249" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="D249" s="0" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C250" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="D250" s="0" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B251" s="1" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C252" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="D252" s="0" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C253" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="D253" s="0" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C254" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="D254" s="0" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C255" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="D255" s="0" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C256" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="D256" s="0" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C257" s="2" t="s">
-        <v>443</v>
-      </c>
-      <c r="D257" s="0" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C258" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="D258" s="0" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C259" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="D259" s="0" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C260" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="D260" s="0" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C261" s="2" t="s">
-        <v>451</v>
-      </c>
-      <c r="D261" s="0" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C262" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="D262" s="0" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C263" s="2" t="s">
-        <v>455</v>
-      </c>
-      <c r="D263" s="0" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C264" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="D264" s="0" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C265" s="2" t="s">
-        <v>459</v>
-      </c>
-      <c r="D265" s="0" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C266" s="2" t="s">
-        <v>461</v>
-      </c>
-      <c r="D266" s="0" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C267" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="D267" s="0" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C268" s="2" t="s">
-        <v>465</v>
-      </c>
-      <c r="D268" s="0" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="269" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B269" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C270" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="D270" s="0" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C271" s="2" t="s">
-        <v>469</v>
-      </c>
-      <c r="D271" s="0" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C272" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="D272" s="0" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B273" s="1" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C274" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="D274" s="0" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C275" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="D275" s="0" t="s">
-        <v>477</v>
-      </c>
     </row>
     <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C276" s="2" t="s">
-        <v>478</v>
-      </c>
-      <c r="D276" s="0" t="s">
+      <c r="B276" s="0" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B277" s="1" t="s">
+      <c r="C277" s="1" t="s">
         <v>480</v>
       </c>
+      <c r="D277" s="0" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C278" s="2" t="s">
-        <v>481</v>
+      <c r="C278" s="1" t="s">
+        <v>482</v>
       </c>
       <c r="D278" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C279" s="2" t="s">
-        <v>483</v>
+      <c r="C279" s="1" t="s">
+        <v>484</v>
       </c>
       <c r="D279" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C280" s="2" t="s">
-        <v>485</v>
-      </c>
-      <c r="D280" s="0" t="s">
+      <c r="B280" s="0" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B281" s="1" t="s">
+      <c r="C281" s="1" t="s">
         <v>487</v>
       </c>
+      <c r="D281" s="0" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C282" s="2" t="s">
-        <v>488</v>
+      <c r="C282" s="1" t="s">
+        <v>489</v>
       </c>
       <c r="D282" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C283" s="2" t="s">
-        <v>490</v>
+      <c r="C283" s="1" t="s">
+        <v>491</v>
       </c>
       <c r="D283" s="0" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B284" s="1" t="s">
         <v>492</v>
       </c>
     </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B284" s="0" t="s">
+        <v>493</v>
+      </c>
+    </row>
     <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C285" s="2" t="s">
-        <v>493</v>
+      <c r="C285" s="1" t="s">
+        <v>494</v>
       </c>
       <c r="D285" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C286" s="2" t="s">
-        <v>495</v>
+      <c r="C286" s="1" t="s">
+        <v>496</v>
       </c>
       <c r="D286" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
     <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C287" s="2" t="s">
-        <v>497</v>
-      </c>
-      <c r="D287" s="0" t="s">
+      <c r="B287" s="0" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C288" s="2" t="s">
+      <c r="C288" s="1" t="s">
         <v>499</v>
       </c>
       <c r="D288" s="0" t="s">
@@ -4245,7 +4868,7 @@
       </c>
     </row>
     <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C289" s="2" t="s">
+      <c r="C289" s="1" t="s">
         <v>501</v>
       </c>
       <c r="D289" s="0" t="s">
@@ -4253,7 +4876,7 @@
       </c>
     </row>
     <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C290" s="2" t="s">
+      <c r="C290" s="1" t="s">
         <v>503</v>
       </c>
       <c r="D290" s="0" t="s">
@@ -4261,7 +4884,7 @@
       </c>
     </row>
     <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C291" s="2" t="s">
+      <c r="C291" s="1" t="s">
         <v>505</v>
       </c>
       <c r="D291" s="0" t="s">
@@ -4269,62 +4892,62 @@
       </c>
     </row>
     <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="1" t="s">
+      <c r="C292" s="1" t="s">
         <v>507</v>
       </c>
+      <c r="D292" s="0" t="s">
+        <v>508</v>
+      </c>
     </row>
     <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B293" s="1" t="s">
-        <v>508</v>
+      <c r="C293" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="D293" s="0" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C294" s="2" t="s">
-        <v>509</v>
+      <c r="C294" s="1" t="s">
+        <v>511</v>
       </c>
       <c r="D294" s="0" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
     </row>
     <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C295" s="2" t="s">
-        <v>511</v>
-      </c>
-      <c r="D295" s="0" t="s">
-        <v>512</v>
+      <c r="A295" s="0" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B296" s="1" t="s">
-        <v>513</v>
+      <c r="B296" s="0" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C297" s="2" t="s">
-        <v>514</v>
+      <c r="C297" s="1" t="s">
+        <v>515</v>
       </c>
       <c r="D297" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C298" s="2" t="s">
-        <v>516</v>
+      <c r="C298" s="1" t="s">
+        <v>517</v>
       </c>
       <c r="D298" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
     </row>
     <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C299" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="D299" s="0" t="s">
+      <c r="B299" s="0" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C300" s="2" t="s">
+      <c r="C300" s="1" t="s">
         <v>520</v>
       </c>
       <c r="D300" s="0" t="s">
@@ -4332,62 +4955,62 @@
       </c>
     </row>
     <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B301" s="1" t="s">
+      <c r="C301" s="1" t="s">
         <v>522</v>
       </c>
+      <c r="D301" s="0" t="s">
+        <v>523</v>
+      </c>
     </row>
     <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C302" s="2" t="s">
-        <v>523</v>
+      <c r="C302" s="1" t="s">
+        <v>524</v>
       </c>
       <c r="D302" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B303" s="1" t="s">
-        <v>524</v>
+      <c r="C303" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="D303" s="0" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C304" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="D304" s="0" t="s">
-        <v>524</v>
+      <c r="B304" s="0" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B305" s="1" t="s">
-        <v>526</v>
+      <c r="C305" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="D305" s="0" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C306" s="2" t="s">
-        <v>527</v>
-      </c>
-      <c r="D306" s="0" t="s">
-        <v>528</v>
+      <c r="B306" s="0" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C307" s="2" t="s">
-        <v>529</v>
+      <c r="C307" s="1" t="s">
+        <v>531</v>
       </c>
       <c r="D307" s="0" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C308" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="D308" s="0" t="s">
+      <c r="B308" s="0" t="s">
         <v>532</v>
       </c>
     </row>
     <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C309" s="2" t="s">
+      <c r="C309" s="1" t="s">
         <v>533</v>
       </c>
       <c r="D309" s="0" t="s">
@@ -4395,7 +5018,7 @@
       </c>
     </row>
     <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C310" s="2" t="s">
+      <c r="C310" s="1" t="s">
         <v>535</v>
       </c>
       <c r="D310" s="0" t="s">
@@ -4403,36 +5026,36 @@
       </c>
     </row>
     <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B311" s="1" t="s">
+      <c r="C311" s="1" t="s">
         <v>537</v>
       </c>
+      <c r="D311" s="0" t="s">
+        <v>538</v>
+      </c>
     </row>
     <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C312" s="2" t="s">
-        <v>538</v>
+      <c r="C312" s="1" t="s">
+        <v>539</v>
       </c>
       <c r="D312" s="0" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
     </row>
     <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C313" s="2" t="s">
-        <v>540</v>
+      <c r="C313" s="1" t="s">
+        <v>541</v>
       </c>
       <c r="D313" s="0" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C314" s="2" t="s">
-        <v>542</v>
-      </c>
-      <c r="D314" s="0" t="s">
+      <c r="B314" s="0" t="s">
         <v>543</v>
       </c>
     </row>
     <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C315" s="2" t="s">
+      <c r="C315" s="1" t="s">
         <v>544</v>
       </c>
       <c r="D315" s="0" t="s">
@@ -4440,68 +5063,68 @@
       </c>
     </row>
     <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C316" s="2" t="s">
+      <c r="C316" s="1" t="s">
         <v>546</v>
       </c>
       <c r="D316" s="0" t="s">
-        <v>409</v>
+        <v>547</v>
       </c>
     </row>
     <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C317" s="2" t="s">
-        <v>547</v>
+      <c r="C317" s="1" t="s">
+        <v>548</v>
       </c>
       <c r="D317" s="0" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C318" s="2" t="s">
-        <v>549</v>
+      <c r="C318" s="1" t="s">
+        <v>550</v>
       </c>
       <c r="D318" s="0" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
     </row>
     <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C319" s="2" t="s">
-        <v>551</v>
+      <c r="C319" s="1" t="s">
+        <v>552</v>
       </c>
       <c r="D319" s="0" t="s">
-        <v>552</v>
+        <v>414</v>
       </c>
     </row>
     <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B320" s="1" t="s">
+      <c r="C320" s="1" t="s">
         <v>553</v>
       </c>
+      <c r="D320" s="0" t="s">
+        <v>554</v>
+      </c>
     </row>
     <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C321" s="2" t="s">
-        <v>554</v>
+      <c r="C321" s="1" t="s">
+        <v>555</v>
       </c>
       <c r="D321" s="0" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C322" s="2" t="s">
-        <v>556</v>
+      <c r="C322" s="1" t="s">
+        <v>557</v>
       </c>
       <c r="D322" s="0" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C323" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="D323" s="0" t="s">
+      <c r="B323" s="0" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C324" s="2" t="s">
+      <c r="C324" s="1" t="s">
         <v>560</v>
       </c>
       <c r="D324" s="0" t="s">
@@ -4509,7 +5132,7 @@
       </c>
     </row>
     <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C325" s="2" t="s">
+      <c r="C325" s="1" t="s">
         <v>562</v>
       </c>
       <c r="D325" s="0" t="s">
@@ -4517,62 +5140,62 @@
       </c>
     </row>
     <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B326" s="1" t="s">
+      <c r="C326" s="1" t="s">
         <v>564</v>
       </c>
+      <c r="D326" s="0" t="s">
+        <v>565</v>
+      </c>
     </row>
     <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C327" s="2" t="s">
-        <v>565</v>
+      <c r="C327" s="1" t="s">
+        <v>566</v>
       </c>
       <c r="D327" s="0" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
     </row>
     <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C328" s="2" t="s">
-        <v>567</v>
+      <c r="C328" s="1" t="s">
+        <v>568</v>
       </c>
       <c r="D328" s="0" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="329" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A329" s="1" t="s">
         <v>569</v>
       </c>
     </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B329" s="0" t="s">
+        <v>570</v>
+      </c>
+    </row>
     <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B330" s="1" t="s">
-        <v>570</v>
+      <c r="C330" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="D330" s="0" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C331" s="2" t="s">
-        <v>571</v>
+      <c r="C331" s="1" t="s">
+        <v>573</v>
       </c>
       <c r="D331" s="0" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
     </row>
     <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C332" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="D332" s="0" t="s">
-        <v>574</v>
+      <c r="A332" s="0" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C333" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="D333" s="0" t="s">
+      <c r="B333" s="0" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C334" s="2" t="s">
+      <c r="C334" s="1" t="s">
         <v>577</v>
       </c>
       <c r="D334" s="0" t="s">
@@ -4580,7 +5203,7 @@
       </c>
     </row>
     <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C335" s="2" t="s">
+      <c r="C335" s="1" t="s">
         <v>579</v>
       </c>
       <c r="D335" s="0" t="s">
@@ -4588,7 +5211,7 @@
       </c>
     </row>
     <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C336" s="2" t="s">
+      <c r="C336" s="1" t="s">
         <v>581</v>
       </c>
       <c r="D336" s="0" t="s">
@@ -4596,7 +5219,7 @@
       </c>
     </row>
     <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C337" s="2" t="s">
+      <c r="C337" s="1" t="s">
         <v>583</v>
       </c>
       <c r="D337" s="0" t="s">
@@ -4604,7 +5227,7 @@
       </c>
     </row>
     <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C338" s="2" t="s">
+      <c r="C338" s="1" t="s">
         <v>585</v>
       </c>
       <c r="D338" s="0" t="s">
@@ -4612,7 +5235,7 @@
       </c>
     </row>
     <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C339" s="2" t="s">
+      <c r="C339" s="1" t="s">
         <v>587</v>
       </c>
       <c r="D339" s="0" t="s">
@@ -4620,7 +5243,7 @@
       </c>
     </row>
     <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C340" s="2" t="s">
+      <c r="C340" s="1" t="s">
         <v>589</v>
       </c>
       <c r="D340" s="0" t="s">
@@ -4628,7 +5251,7 @@
       </c>
     </row>
     <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C341" s="2" t="s">
+      <c r="C341" s="1" t="s">
         <v>591</v>
       </c>
       <c r="D341" s="0" t="s">
@@ -4636,7 +5259,7 @@
       </c>
     </row>
     <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C342" s="2" t="s">
+      <c r="C342" s="1" t="s">
         <v>593</v>
       </c>
       <c r="D342" s="0" t="s">
@@ -4644,290 +5267,345 @@
       </c>
     </row>
     <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B343" s="1" t="s">
+      <c r="C343" s="1" t="s">
         <v>595</v>
       </c>
+      <c r="D343" s="0" t="s">
+        <v>596</v>
+      </c>
     </row>
     <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C344" s="2" t="s">
-        <v>596</v>
+      <c r="C344" s="1" t="s">
+        <v>597</v>
       </c>
       <c r="D344" s="0" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C345" s="2" t="s">
-        <v>598</v>
+      <c r="C345" s="1" t="s">
+        <v>599</v>
       </c>
       <c r="D345" s="0" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
     </row>
     <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C346" s="2" t="s">
-        <v>600</v>
-      </c>
-      <c r="D346" s="0" t="s">
+      <c r="B346" s="0" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C347" s="2" t="s">
+      <c r="C347" s="1" t="s">
         <v>602</v>
       </c>
       <c r="D347" s="0" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="348" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B348" s="1" t="s">
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C348" s="1" t="s">
         <v>604</v>
       </c>
+      <c r="D348" s="0" t="s">
+        <v>605</v>
+      </c>
     </row>
     <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C349" s="2" t="s">
-        <v>605</v>
+      <c r="C349" s="1" t="s">
+        <v>606</v>
       </c>
       <c r="D349" s="0" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C350" s="2" t="s">
-        <v>607</v>
+      <c r="C350" s="1" t="s">
+        <v>608</v>
       </c>
       <c r="D350" s="0" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C351" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="D351" s="0" t="s">
+      <c r="B351" s="0" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C352" s="1" t="s">
+        <v>611</v>
+      </c>
+      <c r="D352" s="0" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C353" s="1" t="s">
+        <v>613</v>
+      </c>
+      <c r="D353" s="0" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C354" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="D354" s="0" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C352" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="D352" s="0" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C353" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="D353" s="0" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C354" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="D354" s="0" t="s">
-        <v>615</v>
-      </c>
-    </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A355" s="1" t="s">
+      <c r="C355" s="1" t="s">
         <v>616</v>
       </c>
+      <c r="D355" s="0" t="s">
+        <v>617</v>
+      </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B356" s="1" t="s">
-        <v>617</v>
+      <c r="C356" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="D356" s="0" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C357" s="2" t="s">
-        <v>618</v>
+      <c r="C357" s="1" t="s">
+        <v>620</v>
       </c>
       <c r="D357" s="0" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
     </row>
     <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C358" s="2" t="s">
-        <v>619</v>
+      <c r="C358" s="1" t="s">
+        <v>622</v>
       </c>
       <c r="D358" s="0" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C359" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="D359" s="0" t="s">
-        <v>622</v>
+      <c r="A359" s="0" t="s">
+        <v>624</v>
       </c>
     </row>
     <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C360" s="2" t="s">
-        <v>623</v>
-      </c>
-      <c r="D360" s="0" t="s">
-        <v>624</v>
+      <c r="B360" s="0" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C361" s="2" t="s">
+      <c r="C361" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="D361" s="0" t="s">
         <v>625</v>
       </c>
-      <c r="D361" s="0" t="s">
-        <v>626</v>
-      </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B362" s="1" t="s">
+      <c r="C362" s="1" t="s">
         <v>627</v>
       </c>
+      <c r="D362" s="0" t="s">
+        <v>628</v>
+      </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C363" s="2" t="s">
-        <v>628</v>
+      <c r="C363" s="1" t="s">
+        <v>629</v>
       </c>
       <c r="D363" s="0" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
     </row>
     <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C364" s="2" t="s">
-        <v>630</v>
+      <c r="C364" s="1" t="s">
+        <v>631</v>
       </c>
       <c r="D364" s="0" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
     </row>
     <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C365" s="2" t="s">
-        <v>632</v>
+      <c r="C365" s="1" t="s">
+        <v>633</v>
       </c>
       <c r="D365" s="0" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C366" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="D366" s="0" t="s">
+      <c r="B366" s="0" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B367" s="1" t="s">
+      <c r="C367" s="1" t="s">
         <v>636</v>
       </c>
+      <c r="D367" s="0" t="s">
+        <v>637</v>
+      </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C368" s="2" t="s">
-        <v>637</v>
+      <c r="C368" s="1" t="s">
+        <v>638</v>
       </c>
       <c r="D368" s="0" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C369" s="2" t="s">
-        <v>639</v>
+      <c r="C369" s="1" t="s">
+        <v>640</v>
       </c>
       <c r="D369" s="0" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B370" s="1" t="s">
-        <v>641</v>
+      <c r="C370" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="D370" s="0" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C371" s="2" t="s">
-        <v>642</v>
-      </c>
-      <c r="D371" s="0" t="s">
-        <v>643</v>
+      <c r="B371" s="0" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C372" s="2" t="s">
-        <v>644</v>
+      <c r="C372" s="1" t="s">
+        <v>645</v>
       </c>
       <c r="D372" s="0" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B373" s="1" t="s">
-        <v>646</v>
+      <c r="C373" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="D373" s="0" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C374" s="2" t="s">
-        <v>647</v>
-      </c>
-      <c r="D374" s="0" t="s">
-        <v>648</v>
+      <c r="B374" s="0" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B375" s="1" t="s">
-        <v>649</v>
+      <c r="C375" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="D375" s="0" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C376" s="2" t="s">
-        <v>650</v>
+      <c r="C376" s="1" t="s">
+        <v>652</v>
       </c>
       <c r="D376" s="0" t="s">
-        <v>649</v>
+        <v>653</v>
       </c>
     </row>
     <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B377" s="1" t="s">
-        <v>651</v>
+      <c r="B377" s="0" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C378" s="2" t="s">
-        <v>652</v>
+      <c r="C378" s="1" t="s">
+        <v>655</v>
       </c>
       <c r="D378" s="0" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
     </row>
     <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B379" s="1" t="s">
-        <v>654</v>
+      <c r="B379" s="0" t="s">
+        <v>657</v>
       </c>
     </row>
     <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C380" s="2" t="s">
-        <v>655</v>
+      <c r="C380" s="1" t="s">
+        <v>658</v>
       </c>
       <c r="D380" s="0" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C381" s="2" t="s">
-        <v>657</v>
-      </c>
-      <c r="D381" s="0" t="s">
-        <v>658</v>
+      <c r="B381" s="0" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C382" s="2" t="s">
-        <v>659</v>
+      <c r="C382" s="1" t="s">
+        <v>660</v>
       </c>
       <c r="D382" s="0" t="s">
-        <v>660</v>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B383" s="0" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C384" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="D384" s="0" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C385" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D385" s="0" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C386" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="D386" s="0" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B391" s="0" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B442" s="0" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="448" customFormat="false" ht="3276.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B448" s="2" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B453" s="0" t="s">
+        <v>672</v>
+      </c>
+      <c r="C453" s="0" t="s">
+        <v>673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>